<commit_message>
I added a couple of views to make queries in SSMS easier to run. I also added Aug. 17 NYSE and NASDAQ files.
</commit_message>
<xml_diff>
--- a/Notes/FieldNotes.xlsx
+++ b/Notes/FieldNotes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\StockData\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08E72912-8BAE-42D8-8E41-CD817AC87F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38EF9A8-839F-4863-B4E3-3FDCD23D7E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{985B1C46-2245-43CE-8270-EF488EA30866}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{985B1C46-2245-43CE-8270-EF488EA30866}"/>
   </bookViews>
   <sheets>
     <sheet name="StockStreak" sheetId="1" r:id="rId1"/>
+    <sheet name="DailyPriceData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Spread</t>
   </si>
@@ -52,6 +53,12 @@
   </si>
   <si>
     <t>100 / Spread * Spread Score</t>
+  </si>
+  <si>
+    <t>Volume Score</t>
+  </si>
+  <si>
+    <t>100 / Average Daily Volume * Volume - 100</t>
   </si>
 </sst>
 </file>
@@ -403,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F2EEB5-DFDB-4A75-AE0B-0D35201B97B5}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -414,6 +421,24 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.796875" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1D80A2-F2F7-4EA7-A28B-4E37C21CB7B8}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.19921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -437,6 +462,14 @@
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>